<commit_message>
feat(task): add base template api
</commit_message>
<xml_diff>
--- a/api/dashboard/task/assets/base_template.xlsx
+++ b/api/dashboard/task/assets/base_template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 mulearn\mulearnbackend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 mulearn\mulearnbackend\api\dashboard\task\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4774EFEA-A337-474A-86DB-42953B7DF9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5580B45C-3968-4079-8AD9-0663D1CA468A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Data Defenitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -410,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
@@ -474,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>